<commit_message>
Besluiten toegevoegd na overleg Hans en Marco
</commit_message>
<xml_diff>
--- a/DCAT-AP-NL-Profile.xlsx
+++ b/DCAT-AP-NL-Profile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcobrattinga/GITREPO/DCAT-AP-NL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5687DFD5-0E00-7149-834A-50C9442B1019}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE51F06F-87F6-C747-AB1E-5DBD2DAF0BE5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="784" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3526" uniqueCount="1617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="1635">
   <si>
     <t>Agent</t>
   </si>
@@ -6320,6 +6320,60 @@
   </si>
   <si>
     <t>De vraag is welke mist. GeoDCAT kent een mapping, mogelijk deze toevoegen als onderdeel van de waardelijst?</t>
+  </si>
+  <si>
+    <t>Besluit overleg H+M</t>
+  </si>
+  <si>
+    <t>Laten zoals het is. In GeoDCAT-AP-NL opnemen dat accessURL verplicht is, plus mapping. Beschrijving aanscherpen obv W3c DCAT 1.1</t>
+  </si>
+  <si>
+    <t>1 waardelijst met 7 waarden. Deze moet je gebruiken als je slechts een URI opgeeft. Je mag er ook een uitwisselgegeven van maken, maar dan moet dan wel voldoen aan het dct:LicenseDocument profielonderdeel</t>
+  </si>
+  <si>
+    <t>MDR waardelijst gebruiken (heeft 3 waarden). Bij GeoDCAT lijken het twee lijstjes: 1 met waarden "other", "no restrictions" en "unknown". Deze valt wel te mappen. De lijst met verwijzingen naar artikel 13 zou dan een aanvullend veld zijn. Marco doet voorstel uitwerking</t>
+  </si>
+  <si>
+    <t>Zie bij issue-12 voor het besluit</t>
+  </si>
+  <si>
+    <t>Waardelijst opnemen zoals GeoDCAT (IANA + GeoDCAT aanvullingen) plus een subset als Waardelijst waarbij je de meeste gebruikten opneemt (We hebben daar nu al een lijstje van). In de beschrijving van dit veld aangeven dat de waarde die je hier gebruikt overeen MOET komen met het mediatype dat je terugkrijgt bij de downloadURL</t>
+  </si>
+  <si>
+    <t>Gedaan</t>
+  </si>
+  <si>
+    <t>We voegen een veld toe waarmee we om kunnen gaan met benoemde tijdsintervallen (bv dc:title). Bij gebruik van een PeriodOfTime zonder begin of einde moet dit veld aanwezig zijn. Bij zoeken worden deze datasets altijd meegenomen, aangezien er dan geen waarde voor is. Probleem is dat schema.org geen uitspraak doet over het datatype. MAAR schema.org lijkt het wel mogelijk te houden om alleen een jaar op te geven, dat kan echter weer niet bij xsd:date. Dus het is OF gewoon een string, OF we beperken het gebruik van de schema.org eigenschappen. Voorlopig beperken tot xsd:date, dit voorleggen aan de groep</t>
+  </si>
+  <si>
+    <t>Met betrekking tot het model: zie issue 43. Geen aanvullend besluit nodig. Tekst wel herschrijven, dan is daarmee dit issue afgedekt.</t>
+  </si>
+  <si>
+    <t>Validatie op het model (actie Marco), en model aanvullen waar nodig conform DCAT-AP-EU</t>
+  </si>
+  <si>
+    <t>We kunnen niet werken met de waardelijst uit Europa, want daar staat niet alles in. Voorstel naar de werkgroep: (a) GeoDCAT-AP oplossing. Dus: het MOET een locatie zijn, dit is een uitwisselgegeven dat MAG een geometrie hebben (bounding box dan wel polygon), OF een link naar de organisatie waar dit het gebied van is</t>
+  </si>
+  <si>
+    <t>Zie besluit bij 7</t>
+  </si>
+  <si>
+    <t>Actie om lijst te maken van de verschillende agent roles en op basis daarvan een beslissing nemen. Belangrijk is dat de semantiek van de rol overeind blijft, met de voorkeur om standaard internationale vocabulaires te gebruiken.</t>
+  </si>
+  <si>
+    <t>Zie besluit bij 58</t>
+  </si>
+  <si>
+    <t>We maken een superwaardelijst die bestaat uit de waardelijsten die gebruikt mogen worden. De superwaardelijst is dan een asset met relaties naar de onderliggende assets. De waarden zitten in deze onderliggende assets. Het is een implementatie-invulling of de waarden uit de superwaardelijst ook opgehaald kunnen worden (dat mag een query zijn, of een gecachte dump, of...)</t>
+  </si>
+  <si>
+    <t>Twee taxonomieen, met mappingen uitwerken en maken. Deze relaties worden dan onderdeel van het profiel. Aandachtspunt is dat volgende week donderdag de redactie bij elkaar zit</t>
+  </si>
+  <si>
+    <t>Zie besluit bij 33</t>
+  </si>
+  <si>
+    <t>Aan CBS (Dennis) vragen welke ontbreken, en deze dan toevoegen aan de waardelijst die we bij DCAT-AP-NL hanteren</t>
   </si>
 </sst>
 </file>
@@ -7891,7 +7945,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -8164,6 +8218,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1227">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -12112,10 +12167,10 @@
   <dimension ref="A1:O94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12525,7 +12580,7 @@
       <c r="E10" s="97" t="s">
         <v>1272</v>
       </c>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="138" t="s">
         <v>1361</v>
       </c>
       <c r="G10" s="96" t="s">
@@ -16579,10 +16634,10 @@
   <dimension ref="A1:I243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A128" sqref="A128"/>
+      <selection pane="bottomRight" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21779,13 +21834,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21799,10 +21854,11 @@
     <col min="8" max="8" width="61.1640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="73.1640625" style="7" customWidth="1"/>
     <col min="10" max="10" width="62.83203125" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="7"/>
+    <col min="11" max="11" width="58" style="37" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>29</v>
       </c>
@@ -21833,8 +21889,11 @@
       <c r="J1" s="6" t="s">
         <v>1604</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="67" customFormat="1" ht="87" x14ac:dyDescent="0.3">
+      <c r="K1" s="4" t="s">
+        <v>1617</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="67" customFormat="1" ht="87" x14ac:dyDescent="0.3">
       <c r="A2" s="51">
         <v>46</v>
       </c>
@@ -21860,8 +21919,9 @@
         <v>1116</v>
       </c>
       <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" s="67" customFormat="1" ht="53" x14ac:dyDescent="0.3">
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" s="67" customFormat="1" ht="53" x14ac:dyDescent="0.3">
       <c r="A3" s="51">
         <v>47</v>
       </c>
@@ -21887,8 +21947,9 @@
         <v>1117</v>
       </c>
       <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" s="67" customFormat="1" ht="206" x14ac:dyDescent="0.3">
+      <c r="K3" s="37"/>
+    </row>
+    <row r="4" spans="1:11" s="67" customFormat="1" ht="206" x14ac:dyDescent="0.3">
       <c r="A4" s="51">
         <v>43</v>
       </c>
@@ -21914,8 +21975,11 @@
         <v>1599</v>
       </c>
       <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" s="67" customFormat="1" ht="53" x14ac:dyDescent="0.3">
+      <c r="K4" s="37" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A5" s="51">
         <v>12</v>
       </c>
@@ -21943,8 +22007,11 @@
       <c r="I5" s="5" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
+      <c r="K5" s="37" t="s">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="67" customFormat="1" ht="87" x14ac:dyDescent="0.3">
       <c r="A6" s="51">
         <v>30</v>
       </c>
@@ -21970,8 +22037,11 @@
         <v>993</v>
       </c>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
+      <c r="K6" s="37" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A7" s="51">
         <v>31</v>
       </c>
@@ -21999,8 +22069,11 @@
       <c r="I7" s="7" t="s">
         <v>1600</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="67" customFormat="1" ht="121" x14ac:dyDescent="0.3">
+      <c r="K7" s="37" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="67" customFormat="1" ht="121" x14ac:dyDescent="0.3">
       <c r="A8" s="51">
         <v>32</v>
       </c>
@@ -22026,8 +22099,11 @@
         <v>993</v>
       </c>
       <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
+      <c r="K8" s="37" t="s">
+        <v>1622</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A9" s="51">
         <v>19</v>
       </c>
@@ -22055,8 +22131,11 @@
       <c r="I9" s="7" t="s">
         <v>991</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" s="67" customFormat="1" ht="189" x14ac:dyDescent="0.3">
+      <c r="K9" s="37" t="s">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="67" customFormat="1" ht="189" x14ac:dyDescent="0.3">
       <c r="A10" s="51">
         <v>50</v>
       </c>
@@ -22080,8 +22159,11 @@
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" s="67" customFormat="1" ht="121" x14ac:dyDescent="0.3">
+      <c r="K10" s="37" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="67" customFormat="1" ht="121" x14ac:dyDescent="0.3">
       <c r="A11" s="55">
         <v>53</v>
       </c>
@@ -22109,8 +22191,11 @@
       <c r="I11" s="8" t="s">
         <v>1601</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="53" x14ac:dyDescent="0.3">
+      <c r="K11" s="37" t="s">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A12" s="51">
         <v>62</v>
       </c>
@@ -22129,8 +22214,11 @@
       <c r="H12" s="5" t="s">
         <v>1602</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="121" x14ac:dyDescent="0.3">
+      <c r="K12" s="37" t="s">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="121" x14ac:dyDescent="0.3">
       <c r="A13" s="51">
         <v>7</v>
       </c>
@@ -22161,8 +22249,11 @@
       <c r="J13" s="5" t="s">
         <v>1603</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="104" x14ac:dyDescent="0.3">
+      <c r="K13" s="37" t="s">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A14" s="51">
         <v>8</v>
       </c>
@@ -22193,8 +22284,11 @@
       <c r="J14" s="7" t="s">
         <v>1605</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="70" x14ac:dyDescent="0.3">
+      <c r="K14" s="37" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A15" s="51">
         <v>15</v>
       </c>
@@ -22225,8 +22319,11 @@
       <c r="J15" s="7" t="s">
         <v>1606</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="27" customFormat="1" ht="104" x14ac:dyDescent="0.3">
+      <c r="K15" s="37" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="27" customFormat="1" ht="104" x14ac:dyDescent="0.3">
       <c r="A16" s="51">
         <v>41</v>
       </c>
@@ -22254,8 +22351,11 @@
       <c r="I16" s="7" t="s">
         <v>1607</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
+      <c r="K16" s="69" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="67" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A17" s="51">
         <v>61</v>
       </c>
@@ -22283,8 +22383,11 @@
       <c r="I17" s="7" t="s">
         <v>1608</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="206" x14ac:dyDescent="0.3">
+      <c r="K17" s="37" t="s">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="206" x14ac:dyDescent="0.3">
       <c r="A18" s="51">
         <v>58</v>
       </c>
@@ -22312,8 +22415,11 @@
       <c r="I18" s="5" t="s">
         <v>1609</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="87" x14ac:dyDescent="0.3">
+      <c r="K18" s="37" t="s">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A19" s="51">
         <v>9</v>
       </c>
@@ -22344,8 +22450,11 @@
       <c r="J19" s="5" t="s">
         <v>1610</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="70" x14ac:dyDescent="0.3">
+      <c r="K19" s="37" t="s">
+        <v>1631</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A20" s="51">
         <v>29</v>
       </c>
@@ -22373,8 +22482,11 @@
       <c r="I20" s="5" t="s">
         <v>1610</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="87" x14ac:dyDescent="0.3">
+      <c r="K20" s="37" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="87" x14ac:dyDescent="0.3">
       <c r="A21" s="51">
         <v>17</v>
       </c>
@@ -22405,8 +22517,11 @@
       <c r="J21" s="5" t="s">
         <v>1611</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="53" x14ac:dyDescent="0.3">
+      <c r="K21" s="37" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A22" s="51">
         <v>51</v>
       </c>
@@ -22434,8 +22549,11 @@
       <c r="I22" s="7" t="s">
         <v>1612</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="70" x14ac:dyDescent="0.3">
+      <c r="K22" s="37" t="s">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A23" s="51">
         <v>33</v>
       </c>
@@ -22463,8 +22581,11 @@
       <c r="I23" s="5" t="s">
         <v>1613</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="121" x14ac:dyDescent="0.3">
+      <c r="K23" s="37" t="s">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="121" x14ac:dyDescent="0.3">
       <c r="A24" s="51">
         <v>10</v>
       </c>
@@ -22495,8 +22616,11 @@
       <c r="J24" s="5" t="s">
         <v>1614</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" s="27" customFormat="1" ht="104" x14ac:dyDescent="0.3">
+      <c r="K24" s="37" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="27" customFormat="1" ht="104" x14ac:dyDescent="0.3">
       <c r="A25" s="51">
         <v>11</v>
       </c>
@@ -22527,8 +22651,11 @@
       <c r="J25" s="27" t="s">
         <v>1615</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" s="27" customFormat="1" ht="53" x14ac:dyDescent="0.3">
+      <c r="K25" s="69" t="s">
+        <v>1633</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="27" customFormat="1" ht="53" x14ac:dyDescent="0.3">
       <c r="A26" s="55">
         <v>54</v>
       </c>
@@ -22556,8 +22683,11 @@
       <c r="I26" s="8" t="s">
         <v>1616</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="53" x14ac:dyDescent="0.3">
+      <c r="K26" s="69" t="s">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A27" s="65">
         <v>5</v>
       </c>
@@ -22586,7 +22716,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="53" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A28" s="65">
         <v>27</v>
       </c>
@@ -22613,7 +22743,7 @@
       </c>
       <c r="I28" s="67"/>
     </row>
-    <row r="29" spans="1:10" ht="70" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A29" s="52">
         <v>28</v>
       </c>
@@ -22640,7 +22770,7 @@
       </c>
       <c r="I29" s="48"/>
     </row>
-    <row r="30" spans="1:10" ht="70" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A30" s="52">
         <v>34</v>
       </c>
@@ -22667,7 +22797,7 @@
       </c>
       <c r="I30" s="48"/>
     </row>
-    <row r="31" spans="1:10" ht="53" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A31" s="52">
         <v>35</v>
       </c>
@@ -22690,7 +22820,7 @@
       <c r="H31" s="47"/>
       <c r="I31" s="48"/>
     </row>
-    <row r="32" spans="1:10" ht="121" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="121" x14ac:dyDescent="0.3">
       <c r="A32" s="52">
         <v>36</v>
       </c>
@@ -22717,7 +22847,7 @@
       </c>
       <c r="I32" s="48"/>
     </row>
-    <row r="33" spans="1:9" ht="53" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A33" s="52">
         <v>37</v>
       </c>
@@ -22742,7 +22872,7 @@
       <c r="H33" s="47"/>
       <c r="I33" s="48"/>
     </row>
-    <row r="34" spans="1:9" s="27" customFormat="1" ht="70" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="27" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A34" s="52">
         <v>38</v>
       </c>
@@ -22768,8 +22898,9 @@
         <v>996</v>
       </c>
       <c r="I34" s="48"/>
-    </row>
-    <row r="35" spans="1:9" ht="138" x14ac:dyDescent="0.3">
+      <c r="K34" s="69"/>
+    </row>
+    <row r="35" spans="1:11" ht="138" x14ac:dyDescent="0.3">
       <c r="A35" s="52">
         <v>39</v>
       </c>
@@ -22796,7 +22927,7 @@
       </c>
       <c r="I35" s="48"/>
     </row>
-    <row r="36" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A36" s="52">
         <v>40</v>
       </c>
@@ -22823,7 +22954,7 @@
       </c>
       <c r="I36" s="48"/>
     </row>
-    <row r="37" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A37" s="52">
         <v>44</v>
       </c>
@@ -22850,7 +22981,7 @@
       </c>
       <c r="I37" s="48"/>
     </row>
-    <row r="38" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A38" s="52">
         <v>52</v>
       </c>
@@ -22877,7 +23008,7 @@
       </c>
       <c r="I38" s="48"/>
     </row>
-    <row r="39" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A39" s="52">
         <v>55</v>
       </c>
@@ -22902,7 +23033,7 @@
       <c r="H39" s="47"/>
       <c r="I39" s="48"/>
     </row>
-    <row r="40" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="65">
         <v>57</v>
       </c>
@@ -22929,7 +23060,7 @@
       </c>
       <c r="I40" s="67"/>
     </row>
-    <row r="41" spans="1:9" ht="104" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A41" s="65">
         <v>1</v>
       </c>
@@ -22958,7 +23089,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="53" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="53" x14ac:dyDescent="0.3">
       <c r="A42" s="52">
         <v>2</v>
       </c>
@@ -22981,7 +23112,7 @@
       </c>
       <c r="I42" s="48"/>
     </row>
-    <row r="43" spans="1:9" ht="104" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A43" s="52">
         <v>3</v>
       </c>
@@ -23010,7 +23141,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="104" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A44" s="65">
         <v>4</v>
       </c>
@@ -23039,7 +23170,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="36" x14ac:dyDescent="0.3">
       <c r="A45" s="52">
         <v>6</v>
       </c>
@@ -23068,7 +23199,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="70" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="70" x14ac:dyDescent="0.3">
       <c r="A46" s="78">
         <v>56</v>
       </c>
@@ -23095,7 +23226,7 @@
       </c>
       <c r="I46" s="77"/>
     </row>
-    <row r="47" spans="1:9" ht="104" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="104" x14ac:dyDescent="0.3">
       <c r="A47" s="65">
         <v>13</v>
       </c>
@@ -23124,7 +23255,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="138" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="138" x14ac:dyDescent="0.3">
       <c r="A48" s="52">
         <v>20</v>
       </c>

</xml_diff>